<commit_message>
Buffing out LDA notebook and add preprocessing scripts
</commit_message>
<xml_diff>
--- a/admin/LDA Results Table.xlsx
+++ b/admin/LDA Results Table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Unigram Strict DF</t>
   </si>
@@ -43,7 +43,28 @@
     <t>Log-Likelihood to Corresponding iTunes Category</t>
   </si>
   <si>
-    <t>Removed stop words</t>
+    <t>Removed podcast stop words</t>
+  </si>
+  <si>
+    <t>removed short words</t>
+  </si>
+  <si>
+    <t>1. Preprocessed</t>
+  </si>
+  <si>
+    <t>2. Model trained</t>
+  </si>
+  <si>
+    <t>3. Categories Mapped to iTunes</t>
+  </si>
+  <si>
+    <t>4. Log-Likelihood calculated</t>
+  </si>
+  <si>
+    <t>iTunes categories weren't well set up. Usubs found junk and then better categorized existing categories. For example …</t>
+  </si>
+  <si>
+    <t>(preprocessing)</t>
   </si>
 </sst>
 </file>
@@ -403,9 +424,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H8"/>
+  <dimension ref="A2:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -416,7 +439,7 @@
     <col min="5" max="5" width="45.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
@@ -427,58 +450,102 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 F5:F8">
+      <formula1>$K$4:$K$10</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added S3 and processed/trained S6
</commit_message>
<xml_diff>
--- a/admin/LDA Results Table.xlsx
+++ b/admin/LDA Results Table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>Unigram Strict DF</t>
   </si>
@@ -64,10 +64,10 @@
     <t>iTunes categories weren't well set up. Usubs found junk and then better categorized existing categories. For example …</t>
   </si>
   <si>
-    <t>(preprocessing)</t>
-  </si>
-  <si>
-    <t>(training</t>
+    <t>(sent to Sam)</t>
+  </si>
+  <si>
+    <t>(need to send to Sam)</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
   <dimension ref="A2:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,10 +473,10 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K4" t="s">
         <v>11</v>
@@ -503,6 +503,9 @@
       <c r="F6" t="s">
         <v>12</v>
       </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
       <c r="K6" t="s">
         <v>13</v>
       </c>
@@ -517,6 +520,9 @@
       <c r="F7" t="s">
         <v>12</v>
       </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
       <c r="K7" t="s">
         <v>14</v>
       </c>
@@ -528,8 +534,11 @@
       <c r="B8" t="s">
         <v>5</v>
       </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -549,7 +558,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 F5:F6 F8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 F5:F6">
       <formula1>$K$4:$K$10</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Moved sub maps and did S1 map
</commit_message>
<xml_diff>
--- a/admin/LDA Results Table.xlsx
+++ b/admin/LDA Results Table.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jblauvelt\Desktop\Projects\podcast_micro_categories\admin\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="240" windowWidth="28380" windowHeight="12465"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Unigram Strict DF</t>
   </si>
@@ -49,28 +54,19 @@
     <t>removed short words</t>
   </si>
   <si>
-    <t>1. Preprocessed</t>
-  </si>
-  <si>
-    <t>2. Model trained</t>
-  </si>
-  <si>
-    <t>3. Categories Mapped to iTunes</t>
-  </si>
-  <si>
-    <t>4. Log-Likelihood calculated</t>
-  </si>
-  <si>
     <t>iTunes categories weren't well set up. Usubs found junk and then better categorized existing categories. For example …</t>
   </si>
   <si>
-    <t>(sent to Sam)</t>
+    <t>Preprocessing</t>
+  </si>
+  <si>
+    <t>Iteration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,11 +113,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -132,6 +136,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -180,7 +187,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -213,9 +220,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -248,6 +272,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -424,63 +465,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K18"/>
+  <dimension ref="A2:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="D3" s="1">
+        <v>49</v>
+      </c>
+      <c r="E3" s="1">
+        <v>603.80999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="D4" s="1">
+        <v>47</v>
+      </c>
+      <c r="E4" s="1">
+        <v>466.13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -489,85 +536,71 @@
       <c r="C5">
         <v>78771</v>
       </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="D5" s="1">
+        <v>45</v>
+      </c>
+      <c r="E5" s="1">
+        <v>516.28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="D6" s="1">
+        <v>40</v>
+      </c>
+      <c r="E6" s="1">
+        <v>466.56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="D7" s="1">
+        <v>44</v>
+      </c>
+      <c r="E7" s="1">
+        <v>498.82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H16" t="s">
+      <c r="D8" s="1">
+        <v>41</v>
+      </c>
+      <c r="E8" s="1">
+        <v>396.41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H17" t="s">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H18" t="s">
-        <v>15</v>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 F5:F6">
-      <formula1>$K$4:$K$10</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>